<commit_message>
Fix bug in drug plate metadata 2.0
</commit_message>
<xml_diff>
--- a/OVP/metadata/plate_layout_v2.0.xlsx
+++ b/OVP/metadata/plate_layout_v2.0.xlsx
@@ -73,52 +73,52 @@
   </si>
   <si>
     <t>patient_1
-Lenvatinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Palbociclib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Abemaciclib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Paclitaxel
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Cobimetinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
 Alpelisib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Osimertinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Lenvatinib + Pembrolizumab
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Durvalumab
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Staurosporine (low) + Etoposide
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Vinblastine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Cediranib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Fluorouracil
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Palbociclib + Letrozole
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Ribociclib
  2</t>
   </si>
   <si>
     <t>patient_1
 Carboplatin + Pembrolizumab
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Osimertinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Mirvetuximab Soravtansine
  3</t>
   </si>
   <si>
@@ -128,98 +128,98 @@
   </si>
   <si>
     <t>patient_1
+Lenvatinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Carboplatin + Pembrolizumab
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+DMSO
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Letrozole
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Palbociclib + Letrozole
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Alpelisib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Niraparib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Alpelisib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Cediranib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Lenvatinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Carboplatin
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Erlotinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Erlotinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
 Olaparib
  1</t>
   </si>
   <si>
     <t>patient_1
-Palbociclib + Letrozole
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-DMSO
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Paclitaxel
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Staurosporine (high) + Etoposide
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Trastuzumab Deruxtecan
- 1</t>
+Gemcitabine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Abemaciclib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Osimertinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Abemaciclib
+ 3</t>
   </si>
   <si>
     <t>patient_1
 Dasatinib
  3</t>
-  </si>
-  <si>
-    <t>patient_1
-Ribociclib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Carboplatin
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Mirvetuximab Soravtansine
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Abemaciclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Olaparib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Ribociclib + Letrozole
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Carboplatin
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Ribociclib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Osimertinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Cyclophosphamide
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Capivasertib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Lenvatinib
- 2</t>
   </si>
   <si>
     <t>patient_1
@@ -228,42 +228,42 @@
   </si>
   <si>
     <t>patient_1
-Erlotinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Trametinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Carboplatin + Pembrolizumab
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Erlotinib
- 3</t>
+Durvalumab
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Everolimus
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Mirvetuximab Soravtansine
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Durvalumab
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Ribociclib + Letrozole
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Carboplatin + Paclitaxel
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Lenvatinib
+ 2</t>
   </si>
   <si>
     <t>patient_1
 Paclitaxel
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Carboplatin + Pembrolizumab
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Niraparib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Capivasertib
  1</t>
   </si>
   <si>
@@ -273,12 +273,27 @@
   </si>
   <si>
     <t>patient_1
-Everolimus
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Fluorouracil
+Dasatinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Mirvetuximab Soravtansine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Carboplatin
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Paclitaxel
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Lenvatinib + Pembrolizumab
  3</t>
   </si>
   <si>
@@ -288,67 +303,52 @@
   </si>
   <si>
     <t>patient_1
+Vinblastine
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Abemaciclib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Cyclophosphamide
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Mirvetuximab Soravtansine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Staurosporine (low) + Etoposide
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Niraparib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
 Ribociclib + Letrozole
  2</t>
   </si>
   <si>
     <t>patient_1
-Capivasertib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Palbociclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Gemcitabine
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Dasatinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Cyclophosphamide
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Mirvetuximab Soravtansine
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Everolimus
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Durvalumab
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
 Trametinib
  2</t>
   </si>
   <si>
     <t>patient_1
-Erlotinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Olaparib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Cobimetinib
+Staurosporine (high) + Etoposide
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Letrozole
  3</t>
   </si>
   <si>
@@ -358,38 +358,38 @@
   </si>
   <si>
     <t>patient_1
+Capivasertib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
 Ribociclib + Letrozole
  3</t>
   </si>
   <si>
     <t>patient_1
-Vinblastine
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Palbociclib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Gemcitabine
+Trastuzumab Deruxtecan
  1</t>
   </si>
   <si>
     <t>patient_1
 Staurosporine (high) + Etoposide
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Durvalumab
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Abemaciclib
- 2</t>
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Osimertinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Trametinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Carboplatin
+ 1</t>
   </si>
   <si>
     <t>patient_1
@@ -398,72 +398,72 @@
   </si>
   <si>
     <t>patient_1
-Cobimetinib
- 2</t>
+Staurosporine (low) + Etoposide
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Gemcitabine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Olaparib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Capivasertib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Fluorouracil
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Trastuzumab Deruxtecan
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Palbociclib
+ 1</t>
   </si>
   <si>
     <t>patient_1
 Cediranib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Letrozole
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Staurosporine (low) + Etoposide
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Carboplatin
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Palbociclib + Letrozole
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Vinblastine
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Lenvatinib + Pembrolizumab
  1</t>
   </si>
   <si>
     <t>patient_1
 Dasatinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Carboplatin + Paclitaxel
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Alpelisib
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Fluorouracil
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Staurosporine (low) + Etoposide
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Letrozole
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Capivasertib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Olaparib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Palbociclib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Cyclophosphamide
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Paclitaxel
  2</t>
   </si>
   <si>
@@ -473,33 +473,33 @@
   </si>
   <si>
     <t>patient_1
-Lenvatinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Cediranib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Cyclophosphamide
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Staurosporine (high) + Etoposide
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Carboplatin + Paclitaxel
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Trametinib
- 1</t>
+Erlotinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Ribociclib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Gemcitabine
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Lenvatinib + Pembrolizumab
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Osimertinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Palbociclib
+ 2</t>
   </si>
   <si>
     <t>patient_1
@@ -508,13 +508,13 @@
   </si>
   <si>
     <t>patient_1
-Lenvatinib + Pembrolizumab
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Cediranib
- 1</t>
+Everolimus
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Carboplatin + Pembrolizumab
+ 2</t>
   </si>
   <si>
     <t>patient_1
@@ -523,17 +523,17 @@
   </si>
   <si>
     <t>patient_1
-Everolimus
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Trastuzumab Deruxtecan
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Durvalumab
+Ribociclib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Staurosporine (high) + Etoposide
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Cyclophosphamide
  3</t>
   </si>
   <si>
@@ -543,17 +543,42 @@
   </si>
   <si>
     <t>patient_1
+Cobimetinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Palbociclib + Letrozole
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+DMSO
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Cobimetinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Fluorouracil
+ 1</t>
+  </si>
+  <si>
+    <t>patient_1
+Letrozole
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
 Trastuzumab Deruxtecan
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Fluorouracil
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-DMSO
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Carboplatin + Paclitaxel
  2</t>
   </si>
   <si>
@@ -563,47 +588,22 @@
   </si>
   <si>
     <t>patient_1
-Staurosporine (low) + Etoposide
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Letrozole
- 1</t>
-  </si>
-  <si>
-    <t>patient_1
-Niraparib
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Palbociclib + Letrozole
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Gemcitabine
- 2</t>
-  </si>
-  <si>
-    <t>patient_1
-Alpelisib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Lenvatinib + Pembrolizumab
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
-Ribociclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_1
 Carboplatin + Paclitaxel
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Cobimetinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_1
+Trametinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_1
+Everolimus
  3</t>
   </si>
   <si>
@@ -733,22 +733,32 @@
   </si>
   <si>
     <t>patient_2
-Trastuzumab Deruxtecan
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Paclitaxel
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Osimertinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Cobimetinib
+Staurosporine (low) + Etoposide
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Lenvatinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Ribociclib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Durvalumab
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Fluorouracil
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Palbociclib
  2</t>
   </si>
   <si>
@@ -758,27 +768,17 @@
   </si>
   <si>
     <t>patient_2
-Cobimetinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Everolimus
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Trastuzumab Deruxtecan
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Alpelisib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Staurosporine (high) + Etoposide
+Capivasertib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Dasatinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Vinblastine
  3</t>
   </si>
   <si>
@@ -788,93 +788,93 @@
   </si>
   <si>
     <t>patient_2
+Letrozole
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Lenvatinib + Pembrolizumab
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+DMSO
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Durvalumab
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Ribociclib + Letrozole
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Carboplatin + Pembrolizumab
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Paclitaxel
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Staurosporine (low) + Etoposide
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Alpelisib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Olaparib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Paclitaxel
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Lenvatinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Gemcitabine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Ribociclib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Capivasertib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
 Palbociclib
  1</t>
   </si>
   <si>
     <t>patient_2
-Abemaciclib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-DMSO
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Trametinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Dasatinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Palbociclib + Letrozole
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Dasatinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Osimertinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Gemcitabine
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Erlotinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Lenvatinib + Pembrolizumab
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Staurosporine (low) + Etoposide
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Ribociclib + Letrozole
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Osimertinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Carboplatin
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Capivasertib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Durvalumab
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Fluorouracil
- 1</t>
+Trastuzumab Deruxtecan
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Ribociclib
+ 3</t>
   </si>
   <si>
     <t>patient_2
@@ -888,42 +888,42 @@
   </si>
   <si>
     <t>patient_2
-Staurosporine (low) + Etoposide
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Carboplatin + Pembrolizumab
- 3</t>
+Fluorouracil
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Palbociclib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Trametinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Everolimus
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Olaparib
+ 1</t>
   </si>
   <si>
     <t>patient_2
 Carboplatin + Paclitaxel
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Gemcitabine
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Cediranib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Alpelisib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Staurosporine (high) + Etoposide
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Dasatinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Palbociclib + Letrozole
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Vinblastine
  1</t>
   </si>
   <si>
@@ -933,83 +933,83 @@
   </si>
   <si>
     <t>patient_2
-Capivasertib
+Paclitaxel
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Osimertinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Abemaciclib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Staurosporine (high) + Etoposide
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Palbociclib + Letrozole
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Niraparib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Cyclophosphamide
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Carboplatin + Pembrolizumab
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Staurosporine (high) + Etoposide
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Staurosporine (low) + Etoposide
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Trametinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Abemaciclib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Osimertinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Erlotinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Carboplatin + Paclitaxel
  2</t>
   </si>
   <si>
     <t>patient_2
 Cediranib
  2</t>
-  </si>
-  <si>
-    <t>patient_2
-Carboplatin + Pembrolizumab
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Palbociclib + Letrozole
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Palbociclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Vinblastine
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Olaparib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Staurosporine (low) + Etoposide
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Lenvatinib + Pembrolizumab
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Palbociclib + Letrozole
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Carboplatin + Paclitaxel
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Lenvatinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Mirvetuximab Soravtansine
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Letrozole
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Carboplatin + Paclitaxel
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Cediranib
- 3</t>
   </si>
   <si>
     <t>patient_2
@@ -1018,7 +1018,7 @@
   </si>
   <si>
     <t>patient_2
-Everolimus
+Gemcitabine
  3</t>
   </si>
   <si>
@@ -1033,7 +1033,7 @@
   </si>
   <si>
     <t>patient_2
-Trametinib
+Trastuzumab Deruxtecan
  1</t>
   </si>
   <si>
@@ -1043,12 +1043,12 @@
   </si>
   <si>
     <t>patient_2
-Vinblastine
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Palbociclib
+Alpelisib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Lenvatinib + Pembrolizumab
  2</t>
   </si>
   <si>
@@ -1058,73 +1058,73 @@
   </si>
   <si>
     <t>patient_2
-Lenvatinib + Pembrolizumab
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Lenvatinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Ribociclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Fluorouracil
- 3</t>
+Mirvetuximab Soravtansine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Gemcitabine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Ribociclib + Letrozole
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Mirvetuximab Soravtansine
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Erlotinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Dasatinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Alpelisib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Trametinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Carboplatin
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Everolimus
+ 1</t>
   </si>
   <si>
     <t>patient_2
 Letrozole
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Alpelisib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Niraparib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Mirvetuximab Soravtansine
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Durvalumab
- 1</t>
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Palbociclib + Letrozole
+ 2</t>
   </si>
   <si>
     <t>patient_2
 Everolimus
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Carboplatin
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Letrozole
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Ribociclib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Erlotinib
- 2</t>
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Trastuzumab Deruxtecan
+ 3</t>
   </si>
   <si>
     <t>patient_2
@@ -1133,17 +1133,17 @@
   </si>
   <si>
     <t>patient_2
-Abemaciclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Paclitaxel
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Mirvetuximab Soravtansine
+Osimertinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Carboplatin + Paclitaxel
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Cediranib
  3</t>
   </si>
   <si>
@@ -1153,13 +1153,13 @@
   </si>
   <si>
     <t>patient_2
-Paclitaxel
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
 Niraparib
- 2</t>
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Ribociclib + Letrozole
+ 1</t>
   </si>
   <si>
     <t>patient_2
@@ -1168,13 +1168,13 @@
   </si>
   <si>
     <t>patient_2
-Ribociclib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Trastuzumab Deruxtecan
- 2</t>
+Mirvetuximab Soravtansine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Dasatinib
+ 1</t>
   </si>
   <si>
     <t>patient_2
@@ -1183,17 +1183,17 @@
   </si>
   <si>
     <t>patient_2
-Fluorouracil
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Vinblastine
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Niraparib
+Cediranib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+Erlotinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Lenvatinib + Pembrolizumab
  3</t>
   </si>
   <si>
@@ -1203,67 +1203,67 @@
   </si>
   <si>
     <t>patient_2
-Ribociclib + Letrozole
- 3</t>
+Capivasertib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Abemaciclib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_2
+DMSO
+ 2</t>
   </si>
   <si>
     <t>patient_2
 Carboplatin + Pembrolizumab
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-DMSO
- 2</t>
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Fluorouracil
+ 1</t>
   </si>
   <si>
     <t>patient_2
 Olaparib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Erlotinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Trametinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Gemcitabine
- 1</t>
-  </si>
-  <si>
-    <t>patient_2
-Abemaciclib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Olaparib
- 2</t>
-  </si>
-  <si>
-    <t>patient_2
-Ribociclib + Letrozole
- 2</t>
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Vinblastine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Cobimetinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Niraparib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Cobimetinib
+ 3</t>
   </si>
   <si>
     <t>patient_2
 Lenvatinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Cyclophosphamide
- 3</t>
-  </si>
-  <si>
-    <t>patient_2
-Capivasertib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_2
+Letrozole
+ 3</t>
+  </si>
+  <si>
+    <t>patient_2
+Carboplatin
  3</t>
   </si>
   <si>
@@ -1279,100 +1279,100 @@
     <t>DMSO</t>
   </si>
   <si>
+    <t>Alpelisib</t>
+  </si>
+  <si>
+    <t>Lenvatinib + Pembrolizumab</t>
+  </si>
+  <si>
+    <t>Durvalumab</t>
+  </si>
+  <si>
+    <t>Staurosporine (low) + Etoposide</t>
+  </si>
+  <si>
+    <t>Vinblastine</t>
+  </si>
+  <si>
+    <t>Cediranib</t>
+  </si>
+  <si>
+    <t>Fluorouracil</t>
+  </si>
+  <si>
+    <t>Palbociclib + Letrozole</t>
+  </si>
+  <si>
+    <t>Ribociclib</t>
+  </si>
+  <si>
+    <t>Carboplatin + Pembrolizumab</t>
+  </si>
+  <si>
     <t>Lenvatinib</t>
   </si>
   <si>
+    <t>Letrozole</t>
+  </si>
+  <si>
+    <t>Niraparib</t>
+  </si>
+  <si>
+    <t>Carboplatin</t>
+  </si>
+  <si>
+    <t>Erlotinib</t>
+  </si>
+  <si>
+    <t>Olaparib</t>
+  </si>
+  <si>
+    <t>Gemcitabine</t>
+  </si>
+  <si>
+    <t>Abemaciclib</t>
+  </si>
+  <si>
+    <t>Osimertinib</t>
+  </si>
+  <si>
+    <t>Dasatinib</t>
+  </si>
+  <si>
+    <t>Everolimus</t>
+  </si>
+  <si>
+    <t>Mirvetuximab Soravtansine</t>
+  </si>
+  <si>
+    <t>Ribociclib + Letrozole</t>
+  </si>
+  <si>
+    <t>Carboplatin + Paclitaxel</t>
+  </si>
+  <si>
+    <t>Paclitaxel</t>
+  </si>
+  <si>
+    <t>Cyclophosphamide</t>
+  </si>
+  <si>
+    <t>Trametinib</t>
+  </si>
+  <si>
+    <t>Staurosporine (high) + Etoposide</t>
+  </si>
+  <si>
+    <t>Capivasertib</t>
+  </si>
+  <si>
+    <t>Trastuzumab Deruxtecan</t>
+  </si>
+  <si>
     <t>Palbociclib</t>
   </si>
   <si>
-    <t>Abemaciclib</t>
-  </si>
-  <si>
-    <t>Paclitaxel</t>
-  </si>
-  <si>
     <t>Cobimetinib</t>
-  </si>
-  <si>
-    <t>Alpelisib</t>
-  </si>
-  <si>
-    <t>Osimertinib</t>
-  </si>
-  <si>
-    <t>Carboplatin + Pembrolizumab</t>
-  </si>
-  <si>
-    <t>Mirvetuximab Soravtansine</t>
-  </si>
-  <si>
-    <t>Olaparib</t>
-  </si>
-  <si>
-    <t>Palbociclib + Letrozole</t>
-  </si>
-  <si>
-    <t>Staurosporine (high) + Etoposide</t>
-  </si>
-  <si>
-    <t>Trastuzumab Deruxtecan</t>
-  </si>
-  <si>
-    <t>Dasatinib</t>
-  </si>
-  <si>
-    <t>Ribociclib</t>
-  </si>
-  <si>
-    <t>Carboplatin</t>
-  </si>
-  <si>
-    <t>Ribociclib + Letrozole</t>
-  </si>
-  <si>
-    <t>Cyclophosphamide</t>
-  </si>
-  <si>
-    <t>Capivasertib</t>
-  </si>
-  <si>
-    <t>Erlotinib</t>
-  </si>
-  <si>
-    <t>Trametinib</t>
-  </si>
-  <si>
-    <t>Niraparib</t>
-  </si>
-  <si>
-    <t>Everolimus</t>
-  </si>
-  <si>
-    <t>Fluorouracil</t>
-  </si>
-  <si>
-    <t>Gemcitabine</t>
-  </si>
-  <si>
-    <t>Durvalumab</t>
-  </si>
-  <si>
-    <t>Vinblastine</t>
-  </si>
-  <si>
-    <t>Cediranib</t>
-  </si>
-  <si>
-    <t>Letrozole</t>
-  </si>
-  <si>
-    <t>Staurosporine (low) + Etoposide</t>
-  </si>
-  <si>
-    <t>Lenvatinib + Pembrolizumab</t>
-  </si>
-  <si>
-    <t>Carboplatin + Paclitaxel</t>
   </si>
   <si>
     <t>Pembrolizumab</t>
@@ -3731,28 +3731,28 @@
         <v>259</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>292</v>
@@ -3764,28 +3764,28 @@
         <v>259</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>276</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="T4" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="60" customHeight="1">
@@ -3796,58 +3796,58 @@
         <v>260</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>275</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>259</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>292</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>259</v>
@@ -3864,55 +3864,55 @@
         <v>259</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>293</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>259</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>269</v>
@@ -3926,28 +3926,28 @@
         <v>262</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>259</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>259</v>
@@ -3956,31 +3956,31 @@
         <v>293</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="P7" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>259</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="60" customHeight="1">
@@ -3991,28 +3991,28 @@
         <v>263</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>259</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>292</v>
@@ -4021,31 +4021,31 @@
         <v>259</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>259</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>261</v>
       </c>
       <c r="U8" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="W8" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="60" customHeight="1">
@@ -4056,61 +4056,61 @@
         <v>264</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>259</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>292</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>259</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="60" customHeight="1">
@@ -4121,61 +4121,61 @@
         <v>265</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>259</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>293</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>259</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="60" customHeight="1">
@@ -4186,28 +4186,28 @@
         <v>266</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>259</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>259</v>
@@ -4216,31 +4216,31 @@
         <v>293</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>259</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="60" customHeight="1">
@@ -4251,28 +4251,28 @@
         <v>267</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>259</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>292</v>
@@ -4281,31 +4281,31 @@
         <v>259</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>259</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="60" customHeight="1">
@@ -4313,64 +4313,64 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>280</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>259</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>285</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>292</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>259</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="60" customHeight="1">
@@ -4378,64 +4378,64 @@
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>259</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>293</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>259</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="60" customHeight="1">
@@ -4446,28 +4446,28 @@
         <v>259</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>259</v>
@@ -4479,28 +4479,28 @@
         <v>259</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="T15" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="U15" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="U15" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="V15" s="1" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="60" customHeight="1">
@@ -4772,7 +4772,7 @@
         <v>294</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>294</v>
@@ -4781,13 +4781,13 @@
         <v>295</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>294</v>
@@ -4796,31 +4796,31 @@
         <v>294</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>296</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>294</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>294</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="60" customHeight="1">
@@ -4831,10 +4831,10 @@
         <v>294</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>294</v>
@@ -4846,7 +4846,7 @@
         <v>294</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>303</v>
@@ -4864,7 +4864,7 @@
         <v>295</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>294</v>
@@ -4873,10 +4873,10 @@
         <v>294</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>294</v>
@@ -4893,31 +4893,31 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>299</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>295</v>
@@ -4938,19 +4938,19 @@
         <v>299</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>295</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>294</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="60" customHeight="1">
@@ -4961,10 +4961,10 @@
         <v>294</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>295</v>
@@ -4976,10 +4976,10 @@
         <v>301</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>295</v>
@@ -4994,28 +4994,28 @@
         <v>295</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>301</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="60" customHeight="1">
@@ -5026,19 +5026,19 @@
         <v>295</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>295</v>
@@ -5056,10 +5056,10 @@
         <v>295</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>295</v>
@@ -5068,7 +5068,7 @@
         <v>295</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>295</v>
@@ -5091,13 +5091,13 @@
         <v>295</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>298</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>295</v>
@@ -5109,7 +5109,7 @@
         <v>295</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>295</v>
@@ -5130,7 +5130,7 @@
         <v>298</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>295</v>
@@ -5139,10 +5139,10 @@
         <v>295</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>295</v>
@@ -5153,16 +5153,16 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>295</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>296</v>
@@ -5174,7 +5174,7 @@
         <v>302</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>296</v>
@@ -5186,19 +5186,19 @@
         <v>299</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>296</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>296</v>
@@ -5210,7 +5210,7 @@
         <v>295</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="60" customHeight="1">
@@ -5218,13 +5218,13 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>296</v>
@@ -5233,16 +5233,16 @@
         <v>300</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>296</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>296</v>
@@ -5275,7 +5275,7 @@
         <v>296</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="60" customHeight="1">

</xml_diff>

<commit_message>
Update OVP plate metadata to include elution control wells
</commit_message>
<xml_diff>
--- a/OVP/metadata/plate_layout_v2.0.xlsx
+++ b/OVP/metadata/plate_layout_v2.0.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\OV_Precision\documents\plate_layout\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FFEA11-2F0D-4594-BF3F-A1B3742F9EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged" sheetId="1" r:id="rId1"/>
@@ -13,12 +19,12 @@
     <sheet name="condition" sheetId="4" r:id="rId4"/>
     <sheet name="replicate" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="317">
   <si>
     <t>A</t>
   </si>
@@ -1422,13 +1428,48 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>elution_ctrl_cycle_00</t>
+  </si>
+  <si>
+    <t>elution_ctrl_cycle_01</t>
+  </si>
+  <si>
+    <t>elution_ctrl_cycle_02</t>
+  </si>
+  <si>
+    <t>elution_ctrl_cycle_03</t>
+  </si>
+  <si>
+    <t>elution_ctrl</t>
+  </si>
+  <si>
+    <t>OVCAR3
+elution_ctrl_cycle_00
+ 1</t>
+  </si>
+  <si>
+    <t>OVCAR3
+elution_ctrl_cycle_01
+ 1</t>
+  </si>
+  <si>
+    <t>OVCAR3
+elution_ctrl_cycle_02
+ 1</t>
+  </si>
+  <si>
+    <t>OVCAR3
+elution_ctrl_cycle_03
+ 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1490,9 +1531,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="15">
     <dxf>
       <border>
         <left style="medium">
@@ -1537,15 +1578,329 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1583,7 +1938,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1617,6 +1972,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1651,9 +2007,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1826,17 +2183,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="25" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="60" customHeight="1">
+    <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -1910,20 +2269,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="60" customHeight="1">
+    <row r="2" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="60" customHeight="1">
+    <row r="3" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" customHeight="1">
+    <row r="4" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1985,10 +2347,13 @@
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="60" customHeight="1">
+    <row r="5" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2050,10 +2415,13 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="60" customHeight="1">
+    <row r="6" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2115,10 +2483,13 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="60" customHeight="1">
+    <row r="7" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2180,7 +2551,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="60" customHeight="1">
+    <row r="8" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2616,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="60" customHeight="1">
+    <row r="9" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2310,7 +2681,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="60" customHeight="1">
+    <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2375,7 +2746,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="60" customHeight="1">
+    <row r="11" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2440,7 +2811,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="60" customHeight="1">
+    <row r="12" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2505,7 +2876,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="60" customHeight="1">
+    <row r="13" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2570,7 +2941,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="60" customHeight="1">
+    <row r="14" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2635,7 +3006,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="60" customHeight="1">
+    <row r="15" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2700,29 +3071,29 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="60" customHeight="1">
+    <row r="16" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="60" customHeight="1">
+    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="14" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="13" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y17">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+    <cfRule type="notContainsErrors" dxfId="12" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2731,17 +3102,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="25" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="60" customHeight="1">
+    <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -2815,20 +3188,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="60" customHeight="1">
+    <row r="2" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="60" customHeight="1">
+    <row r="3" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" customHeight="1">
+    <row r="4" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>256</v>
       </c>
@@ -2890,10 +3266,13 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="60" customHeight="1">
+    <row r="5" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>256</v>
       </c>
@@ -2955,10 +3334,13 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="60" customHeight="1">
+    <row r="6" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>256</v>
       </c>
@@ -3020,10 +3402,13 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="60" customHeight="1">
+    <row r="7" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>256</v>
       </c>
@@ -3085,7 +3470,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="60" customHeight="1">
+    <row r="8" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -3150,7 +3535,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="60" customHeight="1">
+    <row r="9" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -3215,7 +3600,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="60" customHeight="1">
+    <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -3280,7 +3665,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="60" customHeight="1">
+    <row r="11" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -3345,7 +3730,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="60" customHeight="1">
+    <row r="12" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -3410,7 +3795,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="60" customHeight="1">
+    <row r="13" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -3475,7 +3860,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="60" customHeight="1">
+    <row r="14" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -3540,7 +3925,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="60" customHeight="1">
+    <row r="15" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -3605,29 +3990,29 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="60" customHeight="1">
+    <row r="16" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="60" customHeight="1">
+    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="11" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="10" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y17">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+    <cfRule type="notContainsErrors" dxfId="9" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3636,17 +4021,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="25" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="60" customHeight="1">
+    <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -3720,20 +4107,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="60" customHeight="1">
+    <row r="2" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="60" customHeight="1">
+    <row r="3" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" customHeight="1">
+    <row r="4" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>259</v>
       </c>
@@ -3795,10 +4185,13 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="60" customHeight="1">
+    <row r="5" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>259</v>
       </c>
@@ -3860,10 +4253,13 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="60" customHeight="1">
+    <row r="6" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>259</v>
       </c>
@@ -3925,10 +4321,13 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="60" customHeight="1">
+    <row r="7" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>259</v>
       </c>
@@ -3990,7 +4389,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="60" customHeight="1">
+    <row r="8" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -4055,7 +4454,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="60" customHeight="1">
+    <row r="9" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -4120,7 +4519,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="60" customHeight="1">
+    <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -4185,7 +4584,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="60" customHeight="1">
+    <row r="11" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -4250,7 +4649,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="60" customHeight="1">
+    <row r="12" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -4315,7 +4714,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="60" customHeight="1">
+    <row r="13" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -4380,7 +4779,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="60" customHeight="1">
+    <row r="14" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -4445,7 +4844,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="60" customHeight="1">
+    <row r="15" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -4510,29 +4909,29 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="60" customHeight="1">
+    <row r="16" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="60" customHeight="1">
+    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="8" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="7" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y17">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+    <cfRule type="notContainsErrors" dxfId="6" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4541,17 +4940,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="25" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="60" customHeight="1">
+    <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -4625,20 +5026,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="60" customHeight="1">
+    <row r="2" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="60" customHeight="1">
+    <row r="3" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" customHeight="1">
+    <row r="4" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>261</v>
       </c>
@@ -4700,10 +5104,13 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="60" customHeight="1">
+    <row r="5" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>262</v>
       </c>
@@ -4765,10 +5172,13 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="60" customHeight="1">
+    <row r="6" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>263</v>
       </c>
@@ -4830,10 +5240,13 @@
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="60" customHeight="1">
+    <row r="7" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>264</v>
       </c>
@@ -4895,7 +5308,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="60" customHeight="1">
+    <row r="8" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -4960,7 +5373,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="60" customHeight="1">
+    <row r="9" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -5025,7 +5438,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="60" customHeight="1">
+    <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -5090,7 +5503,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="60" customHeight="1">
+    <row r="11" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -5155,7 +5568,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="60" customHeight="1">
+    <row r="12" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -5220,7 +5633,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="60" customHeight="1">
+    <row r="13" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -5285,7 +5698,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="60" customHeight="1">
+    <row r="14" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -5350,7 +5763,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="60" customHeight="1">
+    <row r="15" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -5415,29 +5828,29 @@
         <v>267</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="60" customHeight="1">
+    <row r="16" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="60" customHeight="1">
+    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="5" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="4" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y17">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+    <cfRule type="notContainsErrors" dxfId="3" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5446,17 +5859,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="25" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="60" customHeight="1">
+    <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -5530,20 +5945,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="60" customHeight="1">
+    <row r="2" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="60" customHeight="1">
+    <row r="3" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60" customHeight="1">
+    <row r="4" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>296</v>
       </c>
@@ -5605,10 +6023,13 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="60" customHeight="1">
+    <row r="5" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>296</v>
       </c>
@@ -5670,10 +6091,13 @@
         <v>299</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="60" customHeight="1">
+    <row r="6" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>296</v>
       </c>
@@ -5735,10 +6159,13 @@
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="60" customHeight="1">
+    <row r="7" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>296</v>
       </c>
@@ -5800,7 +6227,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="60" customHeight="1">
+    <row r="8" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -5865,7 +6292,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="60" customHeight="1">
+    <row r="9" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -5930,7 +6357,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="60" customHeight="1">
+    <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -5995,7 +6422,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="60" customHeight="1">
+    <row r="11" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -6060,7 +6487,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="60" customHeight="1">
+    <row r="12" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -6125,7 +6552,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="60" customHeight="1">
+    <row r="13" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -6190,7 +6617,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="60" customHeight="1">
+    <row r="14" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -6255,7 +6682,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="60" customHeight="1">
+    <row r="15" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -6320,19 +6747,19 @@
         <v>297</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="60" customHeight="1">
+    <row r="16" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="60" customHeight="1">
+    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="2" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Change OVP plate layout so that elution control fits with 8-channel pipetting
</commit_message>
<xml_diff>
--- a/OVP/metadata/plate_layout_v2.0.xlsx
+++ b/OVP/metadata/plate_layout_v2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\OV_Precision\documents\plate_layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FFEA11-2F0D-4594-BF3F-A1B3742F9EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A8F4BA-21F7-45FD-832D-450206EC7319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged" sheetId="1" r:id="rId1"/>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,9 +2351,6 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2420,7 +2417,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
@@ -2487,9 +2484,6 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2555,6 +2549,9 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
@@ -2684,6 +2681,9 @@
     <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>22</v>
@@ -3106,7 +3106,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3270,9 +3270,6 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="D5" s="1" t="s">
         <v>256</v>
       </c>
@@ -3406,9 +3403,6 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>256</v>
       </c>
@@ -3474,6 +3468,9 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>256</v>
       </c>
@@ -3603,6 +3600,9 @@
     <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>256</v>
@@ -4025,7 +4025,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,9 +4189,6 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="D5" s="1" t="s">
         <v>259</v>
       </c>
@@ -4325,9 +4322,6 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>259</v>
       </c>
@@ -4393,6 +4387,9 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>259</v>
       </c>
@@ -4522,6 +4519,9 @@
     <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>259</v>
@@ -4944,7 +4944,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5108,9 +5108,6 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="D5" s="1" t="s">
         <v>262</v>
       </c>
@@ -5177,7 +5174,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>263</v>
@@ -5244,9 +5241,6 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>264</v>
       </c>
@@ -5312,6 +5306,9 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>265</v>
       </c>
@@ -5441,6 +5438,9 @@
     <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>267</v>
@@ -5862,8 +5862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6027,9 +6027,6 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="D5" s="1" t="s">
         <v>296</v>
       </c>
@@ -6163,9 +6160,6 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>296</v>
       </c>
@@ -6231,6 +6225,9 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>296</v>
       </c>
@@ -6360,6 +6357,9 @@
     <row r="10" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>297</v>

</xml_diff>